<commit_message>
CIERRE DEL 2 DE DIC 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 10  OCTUBRE 2021/CREDITOS  4 CARNES  11 SUR   OCTUBRE       2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 10  OCTUBRE 2021/CREDITOS  4 CARNES  11 SUR   OCTUBRE       2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rouss\Documents\GitHub\TRABAJO\01 DOCUEMENTOS\CENTRAL  ARCHIVO  2 0 2 1\CENTRAL # 10  OCTUBRE 2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A325592C-BBD2-4133-A63F-EC1AF1131C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4726101-2842-4480-9881-E3FA3CACA187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7380" yWindow="195" windowWidth="12960" windowHeight="10920" firstSheet="9" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2985" yWindow="0" windowWidth="12240" windowHeight="10920" firstSheet="9" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="E N E R O    2 0 2 1 " sheetId="1" r:id="rId1"/>
@@ -138,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="91">
   <si>
     <t xml:space="preserve">ABASTO 4 CARNES </t>
   </si>
@@ -626,7 +626,7 @@
     <numFmt numFmtId="165" formatCode="[$-C0A]d\-mmm\-yy;@"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -832,6 +832,14 @@
       <b/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000099"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1351,7 +1359,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="239">
+  <cellXfs count="241">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1895,6 +1903,20 @@
     </xf>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1937,20 +1959,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="27" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="27" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -1960,6 +1972,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF000099"/>
       <color rgb="FF0000FF"/>
       <color rgb="FFFF00FF"/>
       <color rgb="FF00FF00"/>
@@ -1969,7 +1982,6 @@
       <color rgb="FF66FFFF"/>
       <color rgb="FF9966FF"/>
       <color rgb="FFFF99FF"/>
-      <color rgb="FF99CCFF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -3478,25 +3490,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="219" t="s">
+      <c r="B1" s="225" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="220"/>
-      <c r="D1" s="220"/>
-      <c r="E1" s="220"/>
-      <c r="F1" s="220"/>
-      <c r="G1" s="221"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="227"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="222" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="222"/>
-      <c r="D2" s="222"/>
-      <c r="E2" s="222"/>
-      <c r="F2" s="222"/>
+      <c r="B2" s="228" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="228"/>
+      <c r="D2" s="228"/>
+      <c r="E2" s="228"/>
+      <c r="F2" s="228"/>
       <c r="G2" s="77"/>
       <c r="H2" s="4"/>
       <c r="I2" s="2"/>
@@ -5796,12 +5808,12 @@
       <c r="B89" s="36"/>
       <c r="C89" s="36"/>
       <c r="D89" s="2"/>
-      <c r="E89" s="223">
+      <c r="E89" s="229">
         <f>E85-G85</f>
         <v>0</v>
       </c>
-      <c r="F89" s="224"/>
-      <c r="G89" s="225"/>
+      <c r="F89" s="230"/>
+      <c r="G89" s="231"/>
       <c r="I89" s="2"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -5817,11 +5829,11 @@
       <c r="B91" s="36"/>
       <c r="C91" s="36"/>
       <c r="D91" s="2"/>
-      <c r="E91" s="226" t="s">
+      <c r="E91" s="232" t="s">
         <v>10</v>
       </c>
-      <c r="F91" s="226"/>
-      <c r="G91" s="226"/>
+      <c r="F91" s="232"/>
+      <c r="G91" s="232"/>
       <c r="I91" s="2"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -5943,8 +5955,8 @@
   </sheetPr>
   <dimension ref="A1:Q173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5963,25 +5975,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="219" t="s">
+      <c r="B1" s="225" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="220"/>
-      <c r="D1" s="220"/>
-      <c r="E1" s="220"/>
-      <c r="F1" s="220"/>
-      <c r="G1" s="221"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="227"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="222" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="222"/>
-      <c r="D2" s="222"/>
-      <c r="E2" s="222"/>
-      <c r="F2" s="222"/>
+      <c r="B2" s="228" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="228"/>
+      <c r="D2" s="228"/>
+      <c r="E2" s="228"/>
+      <c r="F2" s="228"/>
       <c r="G2" s="77"/>
       <c r="H2" s="4"/>
       <c r="I2" s="2"/>
@@ -6025,11 +6037,15 @@
       <c r="E4" s="19">
         <v>52</v>
       </c>
-      <c r="F4" s="47"/>
-      <c r="G4" s="25"/>
+      <c r="F4" s="47">
+        <v>44480</v>
+      </c>
+      <c r="G4" s="25">
+        <v>52</v>
+      </c>
       <c r="H4" s="16">
         <f t="shared" ref="H4:H155" si="0">E4-G4</f>
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="I4" s="2"/>
     </row>
@@ -6148,13 +6164,13 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="233"/>
-      <c r="B10" s="234">
+      <c r="A10" s="219"/>
+      <c r="B10" s="220">
         <f t="shared" si="1"/>
         <v>2564</v>
       </c>
-      <c r="C10" s="235"/>
-      <c r="D10" s="236" t="s">
+      <c r="C10" s="221"/>
+      <c r="D10" s="222" t="s">
         <v>87</v>
       </c>
       <c r="E10" s="20"/>
@@ -6166,13 +6182,13 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="233"/>
-      <c r="B11" s="234">
+      <c r="A11" s="219"/>
+      <c r="B11" s="220">
         <f t="shared" si="1"/>
         <v>2565</v>
       </c>
-      <c r="C11" s="235"/>
-      <c r="D11" s="236" t="s">
+      <c r="C11" s="221"/>
+      <c r="D11" s="222" t="s">
         <v>87</v>
       </c>
       <c r="E11" s="20"/>
@@ -6184,13 +6200,13 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="233"/>
-      <c r="B12" s="234">
+      <c r="A12" s="219"/>
+      <c r="B12" s="220">
         <f t="shared" si="1"/>
         <v>2566</v>
       </c>
       <c r="C12" s="23"/>
-      <c r="D12" s="236" t="s">
+      <c r="D12" s="222" t="s">
         <v>87</v>
       </c>
       <c r="E12" s="20"/>
@@ -6202,13 +6218,13 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="233"/>
-      <c r="B13" s="234">
+      <c r="A13" s="219"/>
+      <c r="B13" s="220">
         <f t="shared" si="1"/>
         <v>2567</v>
       </c>
-      <c r="C13" s="237"/>
-      <c r="D13" s="236" t="s">
+      <c r="C13" s="223"/>
+      <c r="D13" s="222" t="s">
         <v>87</v>
       </c>
       <c r="E13" s="20"/>
@@ -6220,15 +6236,15 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="233">
+      <c r="A14" s="219">
         <v>44472</v>
       </c>
-      <c r="B14" s="234">
+      <c r="B14" s="220">
         <f t="shared" si="1"/>
         <v>2568</v>
       </c>
       <c r="C14" s="23"/>
-      <c r="D14" s="238" t="s">
+      <c r="D14" s="224" t="s">
         <v>86</v>
       </c>
       <c r="E14" s="20">
@@ -6246,15 +6262,15 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="233">
+      <c r="A15" s="219">
         <v>44472</v>
       </c>
-      <c r="B15" s="234">
+      <c r="B15" s="220">
         <f t="shared" si="1"/>
         <v>2569</v>
       </c>
-      <c r="C15" s="237"/>
-      <c r="D15" s="236" t="s">
+      <c r="C15" s="223"/>
+      <c r="D15" s="222" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="20">
@@ -6308,11 +6324,15 @@
       <c r="E17" s="20">
         <v>37880</v>
       </c>
-      <c r="F17" s="49"/>
-      <c r="G17" s="27"/>
+      <c r="F17" s="49">
+        <v>44478</v>
+      </c>
+      <c r="G17" s="27">
+        <v>37880</v>
+      </c>
       <c r="H17" s="16">
         <f t="shared" si="0"/>
-        <v>37880</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -6382,11 +6402,15 @@
       <c r="E20" s="20">
         <v>91</v>
       </c>
-      <c r="F20" s="49"/>
-      <c r="G20" s="27"/>
+      <c r="F20" s="49">
+        <v>44480</v>
+      </c>
+      <c r="G20" s="27">
+        <v>91</v>
+      </c>
       <c r="H20" s="16">
         <f t="shared" si="0"/>
-        <v>91</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -6430,11 +6454,15 @@
       <c r="E22" s="20">
         <v>2083</v>
       </c>
-      <c r="F22" s="49"/>
-      <c r="G22" s="27"/>
+      <c r="F22" s="49">
+        <v>44480</v>
+      </c>
+      <c r="G22" s="27">
+        <v>2083</v>
+      </c>
       <c r="H22" s="16">
         <f t="shared" si="0"/>
-        <v>2083</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -6478,11 +6506,15 @@
       <c r="E24" s="20">
         <v>5699</v>
       </c>
-      <c r="F24" s="49"/>
-      <c r="G24" s="27"/>
+      <c r="F24" s="49">
+        <v>44480</v>
+      </c>
+      <c r="G24" s="27">
+        <v>5699</v>
+      </c>
       <c r="H24" s="16">
         <f t="shared" si="0"/>
-        <v>5699</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -6500,11 +6532,15 @@
       <c r="E25" s="20">
         <v>743</v>
       </c>
-      <c r="F25" s="49"/>
-      <c r="G25" s="27"/>
+      <c r="F25" s="49">
+        <v>44477</v>
+      </c>
+      <c r="G25" s="27">
+        <v>743</v>
+      </c>
       <c r="H25" s="16">
         <f t="shared" si="0"/>
-        <v>743</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -6548,11 +6584,15 @@
       <c r="E27" s="20">
         <v>65</v>
       </c>
-      <c r="F27" s="49"/>
-      <c r="G27" s="27"/>
+      <c r="F27" s="49">
+        <v>44480</v>
+      </c>
+      <c r="G27" s="27">
+        <v>65</v>
+      </c>
       <c r="H27" s="16">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -6592,11 +6632,15 @@
       <c r="E29" s="20">
         <v>7622</v>
       </c>
-      <c r="F29" s="49"/>
-      <c r="G29" s="27"/>
+      <c r="F29" s="49">
+        <v>44477</v>
+      </c>
+      <c r="G29" s="27">
+        <v>7622</v>
+      </c>
       <c r="H29" s="16">
         <f t="shared" si="0"/>
-        <v>7622</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -6614,235 +6658,351 @@
       <c r="E30" s="20">
         <v>1735</v>
       </c>
-      <c r="F30" s="49"/>
-      <c r="G30" s="27"/>
+      <c r="F30" s="49">
+        <v>44477</v>
+      </c>
+      <c r="G30" s="27">
+        <v>1736</v>
+      </c>
       <c r="H30" s="16">
         <f t="shared" si="0"/>
-        <v>1735</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
+      <c r="A31" s="11">
+        <v>44477</v>
+      </c>
       <c r="B31" s="12">
         <f t="shared" si="1"/>
         <v>2585</v>
       </c>
       <c r="C31" s="21"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="49"/>
-      <c r="G31" s="27"/>
+      <c r="D31" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" s="20">
+        <v>1960</v>
+      </c>
+      <c r="F31" s="49">
+        <v>44478</v>
+      </c>
+      <c r="G31" s="27">
+        <v>1960</v>
+      </c>
       <c r="H31" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
+      <c r="A32" s="11">
+        <v>44477</v>
+      </c>
       <c r="B32" s="12">
         <f t="shared" si="1"/>
         <v>2586</v>
       </c>
       <c r="C32" s="21"/>
-      <c r="D32" s="43"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="49"/>
-      <c r="G32" s="27"/>
+      <c r="D32" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="20">
+        <v>1684</v>
+      </c>
+      <c r="F32" s="49">
+        <v>44478</v>
+      </c>
+      <c r="G32" s="27">
+        <v>1684</v>
+      </c>
       <c r="H32" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
+      <c r="A33" s="11">
+        <v>44477</v>
+      </c>
       <c r="B33" s="12">
         <f t="shared" si="1"/>
         <v>2587</v>
       </c>
       <c r="C33" s="21"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="49"/>
-      <c r="G33" s="27"/>
+      <c r="D33" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" s="20">
+        <v>6986</v>
+      </c>
+      <c r="F33" s="49">
+        <v>44478</v>
+      </c>
+      <c r="G33" s="27">
+        <v>6986</v>
+      </c>
       <c r="H33" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="11"/>
+      <c r="A34" s="11">
+        <v>44477</v>
+      </c>
       <c r="B34" s="12">
         <f t="shared" si="1"/>
         <v>2588</v>
       </c>
       <c r="C34" s="22"/>
-      <c r="D34" s="43"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="49"/>
-      <c r="G34" s="27"/>
+      <c r="D34" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34" s="20">
+        <v>1905</v>
+      </c>
+      <c r="F34" s="49">
+        <v>44478</v>
+      </c>
+      <c r="G34" s="27">
+        <v>1905</v>
+      </c>
       <c r="H34" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
+      <c r="A35" s="11">
+        <v>44478</v>
+      </c>
       <c r="B35" s="12">
         <f t="shared" si="1"/>
         <v>2589</v>
       </c>
       <c r="C35" s="23"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="20"/>
+      <c r="D35" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="E35" s="20">
+        <v>35026</v>
+      </c>
       <c r="F35" s="49"/>
       <c r="G35" s="27"/>
       <c r="H35" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>35026</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="11"/>
+      <c r="A36" s="11">
+        <v>44478</v>
+      </c>
       <c r="B36" s="12">
         <f t="shared" si="1"/>
         <v>2590</v>
       </c>
       <c r="C36" s="21"/>
-      <c r="D36" s="43"/>
-      <c r="E36" s="20"/>
+      <c r="D36" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" s="20">
+        <v>4301</v>
+      </c>
       <c r="F36" s="49"/>
       <c r="G36" s="27"/>
       <c r="H36" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4301</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="11"/>
+      <c r="A37" s="11">
+        <v>44478</v>
+      </c>
       <c r="B37" s="12">
         <f t="shared" si="1"/>
         <v>2591</v>
       </c>
       <c r="C37" s="21"/>
-      <c r="D37" s="43"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="27"/>
+      <c r="D37" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="E37" s="20">
+        <v>13917</v>
+      </c>
+      <c r="F37" s="49">
+        <v>44479</v>
+      </c>
+      <c r="G37" s="27">
+        <v>13917</v>
+      </c>
       <c r="H37" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="11"/>
+      <c r="A38" s="11">
+        <v>44479</v>
+      </c>
       <c r="B38" s="12">
         <f t="shared" si="1"/>
         <v>2592</v>
       </c>
       <c r="C38" s="21"/>
-      <c r="D38" s="43"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="49"/>
-      <c r="G38" s="27"/>
+      <c r="D38" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="E38" s="20">
+        <v>1023</v>
+      </c>
+      <c r="F38" s="49">
+        <v>44481</v>
+      </c>
+      <c r="G38" s="27">
+        <v>1023</v>
+      </c>
       <c r="H38" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="11"/>
+      <c r="A39" s="11">
+        <v>44479</v>
+      </c>
       <c r="B39" s="12">
         <f t="shared" si="1"/>
         <v>2593</v>
       </c>
       <c r="C39" s="21"/>
-      <c r="D39" s="43"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="49"/>
-      <c r="G39" s="27"/>
+      <c r="D39" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="E39" s="20">
+        <v>1905</v>
+      </c>
+      <c r="F39" s="49">
+        <v>44481</v>
+      </c>
+      <c r="G39" s="27">
+        <v>1905</v>
+      </c>
       <c r="H39" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="11"/>
+      <c r="A40" s="11">
+        <v>44480</v>
+      </c>
       <c r="B40" s="12">
         <f t="shared" si="1"/>
         <v>2594</v>
       </c>
       <c r="C40" s="21"/>
-      <c r="D40" s="43"/>
-      <c r="E40" s="20"/>
+      <c r="D40" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="E40" s="20">
+        <v>7053</v>
+      </c>
       <c r="F40" s="49"/>
       <c r="G40" s="27"/>
       <c r="H40" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7053</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="11"/>
+      <c r="A41" s="11">
+        <v>44480</v>
+      </c>
       <c r="B41" s="12">
         <f t="shared" si="1"/>
         <v>2595</v>
       </c>
       <c r="C41" s="21"/>
-      <c r="D41" s="43"/>
-      <c r="E41" s="20"/>
+      <c r="D41" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="E41" s="20">
+        <v>2578</v>
+      </c>
       <c r="F41" s="49"/>
       <c r="G41" s="27"/>
       <c r="H41" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2578</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="11"/>
+      <c r="A42" s="11">
+        <v>44480</v>
+      </c>
       <c r="B42" s="12">
         <f t="shared" si="1"/>
         <v>2596</v>
       </c>
       <c r="C42" s="21"/>
-      <c r="D42" s="43"/>
-      <c r="E42" s="20"/>
+      <c r="D42" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="E42" s="20">
+        <v>5531</v>
+      </c>
       <c r="F42" s="49"/>
       <c r="G42" s="27"/>
       <c r="H42" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5531</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="11"/>
+      <c r="A43" s="11">
+        <v>44480</v>
+      </c>
       <c r="B43" s="12">
         <f t="shared" si="1"/>
         <v>2597</v>
       </c>
       <c r="C43" s="21"/>
-      <c r="D43" s="43"/>
-      <c r="E43" s="20"/>
+      <c r="D43" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43" s="20">
+        <v>3988</v>
+      </c>
       <c r="F43" s="49"/>
       <c r="G43" s="27"/>
       <c r="H43" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3988</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="11"/>
+      <c r="A44" s="11">
+        <v>44481</v>
+      </c>
       <c r="B44" s="12">
         <f t="shared" si="1"/>
         <v>2598</v>
       </c>
       <c r="C44" s="21"/>
-      <c r="D44" s="43"/>
-      <c r="E44" s="20"/>
+      <c r="D44" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="E44" s="20">
+        <v>10473</v>
+      </c>
       <c r="F44" s="49"/>
       <c r="G44" s="27"/>
       <c r="H44" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10473</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8699,16 +8859,16 @@
       <c r="D156" s="2"/>
       <c r="E156" s="37">
         <f>SUM(E4:E155)</f>
-        <v>187057</v>
+        <v>285387</v>
       </c>
       <c r="F156" s="37"/>
       <c r="G156" s="37">
         <f>SUM(G4:G155)</f>
-        <v>70986</v>
+        <v>156337</v>
       </c>
       <c r="H156" s="38">
         <f>SUM(H4:H155)</f>
-        <v>116071</v>
+        <v>129050</v>
       </c>
       <c r="I156" s="2"/>
     </row>
@@ -8750,12 +8910,12 @@
       <c r="B160" s="165"/>
       <c r="C160" s="36"/>
       <c r="D160" s="2"/>
-      <c r="E160" s="223">
+      <c r="E160" s="229">
         <f>E156-G156</f>
-        <v>116071</v>
-      </c>
-      <c r="F160" s="224"/>
-      <c r="G160" s="225"/>
+        <v>129050</v>
+      </c>
+      <c r="F160" s="230"/>
+      <c r="G160" s="231"/>
       <c r="I160" s="2"/>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
@@ -8771,11 +8931,11 @@
       <c r="B162" s="165"/>
       <c r="C162" s="36"/>
       <c r="D162" s="2"/>
-      <c r="E162" s="226" t="s">
+      <c r="E162" s="232" t="s">
         <v>10</v>
       </c>
-      <c r="F162" s="226"/>
-      <c r="G162" s="226"/>
+      <c r="F162" s="232"/>
+      <c r="G162" s="232"/>
       <c r="I162" s="2"/>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
@@ -8942,19 +9102,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="227" t="s">
+      <c r="C1" s="233" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="228"/>
-      <c r="E1" s="228"/>
+      <c r="D1" s="234"/>
+      <c r="E1" s="234"/>
       <c r="F1" s="208" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="227" t="s">
+      <c r="J1" s="233" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="228"/>
-      <c r="L1" s="228"/>
+      <c r="K1" s="234"/>
+      <c r="L1" s="234"/>
     </row>
     <row r="2" spans="1:14" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="50"/>
@@ -11296,10 +11456,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="229" t="s">
+      <c r="B1" s="235" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="230"/>
+      <c r="C1" s="236"/>
       <c r="D1" s="113"/>
     </row>
     <row r="2" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -11319,10 +11479,10 @@
       <c r="F2" s="112" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="231" t="s">
+      <c r="G2" s="237" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="232"/>
+      <c r="H2" s="238"/>
     </row>
     <row r="3" spans="1:8" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="65">
@@ -11588,25 +11748,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="219" t="s">
+      <c r="B1" s="225" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="220"/>
-      <c r="D1" s="220"/>
-      <c r="E1" s="220"/>
-      <c r="F1" s="220"/>
-      <c r="G1" s="221"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="227"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="222" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="222"/>
-      <c r="D2" s="222"/>
-      <c r="E2" s="222"/>
-      <c r="F2" s="222"/>
+      <c r="B2" s="228" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="228"/>
+      <c r="D2" s="228"/>
+      <c r="E2" s="228"/>
+      <c r="F2" s="228"/>
       <c r="G2" s="77"/>
       <c r="H2" s="4"/>
       <c r="I2" s="2"/>
@@ -13979,12 +14139,12 @@
       <c r="B95" s="36"/>
       <c r="C95" s="36"/>
       <c r="D95" s="2"/>
-      <c r="E95" s="223">
+      <c r="E95" s="229">
         <f>E91-G91</f>
         <v>0</v>
       </c>
-      <c r="F95" s="224"/>
-      <c r="G95" s="225"/>
+      <c r="F95" s="230"/>
+      <c r="G95" s="231"/>
       <c r="I95" s="2"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -14000,11 +14160,11 @@
       <c r="B97" s="36"/>
       <c r="C97" s="36"/>
       <c r="D97" s="2"/>
-      <c r="E97" s="226" t="s">
+      <c r="E97" s="232" t="s">
         <v>10</v>
       </c>
-      <c r="F97" s="226"/>
-      <c r="G97" s="226"/>
+      <c r="F97" s="232"/>
+      <c r="G97" s="232"/>
       <c r="I97" s="2"/>
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.25">
@@ -14147,25 +14307,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="219" t="s">
+      <c r="B1" s="225" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="220"/>
-      <c r="D1" s="220"/>
-      <c r="E1" s="220"/>
-      <c r="F1" s="220"/>
-      <c r="G1" s="221"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="227"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="222" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="222"/>
-      <c r="D2" s="222"/>
-      <c r="E2" s="222"/>
-      <c r="F2" s="222"/>
+      <c r="B2" s="228" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="228"/>
+      <c r="D2" s="228"/>
+      <c r="E2" s="228"/>
+      <c r="F2" s="228"/>
       <c r="G2" s="77"/>
       <c r="H2" s="4"/>
       <c r="I2" s="2"/>
@@ -17322,12 +17482,12 @@
       <c r="B124" s="36"/>
       <c r="C124" s="36"/>
       <c r="D124" s="2"/>
-      <c r="E124" s="223">
+      <c r="E124" s="229">
         <f>E120-G120</f>
         <v>0</v>
       </c>
-      <c r="F124" s="224"/>
-      <c r="G124" s="225"/>
+      <c r="F124" s="230"/>
+      <c r="G124" s="231"/>
       <c r="I124" s="2"/>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
@@ -17343,11 +17503,11 @@
       <c r="B126" s="36"/>
       <c r="C126" s="36"/>
       <c r="D126" s="2"/>
-      <c r="E126" s="226" t="s">
+      <c r="E126" s="232" t="s">
         <v>10</v>
       </c>
-      <c r="F126" s="226"/>
-      <c r="G126" s="226"/>
+      <c r="F126" s="232"/>
+      <c r="G126" s="232"/>
       <c r="I126" s="2"/>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
@@ -17488,25 +17648,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="219" t="s">
+      <c r="B1" s="225" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="220"/>
-      <c r="D1" s="220"/>
-      <c r="E1" s="220"/>
-      <c r="F1" s="220"/>
-      <c r="G1" s="221"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="227"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="222" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="222"/>
-      <c r="D2" s="222"/>
-      <c r="E2" s="222"/>
-      <c r="F2" s="222"/>
+      <c r="B2" s="228" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="228"/>
+      <c r="D2" s="228"/>
+      <c r="E2" s="228"/>
+      <c r="F2" s="228"/>
       <c r="G2" s="77"/>
       <c r="H2" s="4"/>
       <c r="I2" s="2"/>
@@ -19951,12 +20111,12 @@
       <c r="B97" s="36"/>
       <c r="C97" s="36"/>
       <c r="D97" s="2"/>
-      <c r="E97" s="223">
+      <c r="E97" s="229">
         <f>E93-G93</f>
         <v>0</v>
       </c>
-      <c r="F97" s="224"/>
-      <c r="G97" s="225"/>
+      <c r="F97" s="230"/>
+      <c r="G97" s="231"/>
       <c r="I97" s="2"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -19972,11 +20132,11 @@
       <c r="B99" s="36"/>
       <c r="C99" s="36"/>
       <c r="D99" s="2"/>
-      <c r="E99" s="226" t="s">
+      <c r="E99" s="232" t="s">
         <v>10</v>
       </c>
-      <c r="F99" s="226"/>
-      <c r="G99" s="226"/>
+      <c r="F99" s="232"/>
+      <c r="G99" s="232"/>
       <c r="I99" s="2"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -20125,25 +20285,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="219" t="s">
+      <c r="B1" s="225" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="220"/>
-      <c r="D1" s="220"/>
-      <c r="E1" s="220"/>
-      <c r="F1" s="220"/>
-      <c r="G1" s="221"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="227"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="222" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="222"/>
-      <c r="D2" s="222"/>
-      <c r="E2" s="222"/>
-      <c r="F2" s="222"/>
+      <c r="B2" s="228" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="228"/>
+      <c r="D2" s="228"/>
+      <c r="E2" s="228"/>
+      <c r="F2" s="228"/>
       <c r="G2" s="77"/>
       <c r="H2" s="4"/>
       <c r="I2" s="2"/>
@@ -23277,12 +23437,12 @@
       <c r="B125" s="165"/>
       <c r="C125" s="36"/>
       <c r="D125" s="2"/>
-      <c r="E125" s="223">
+      <c r="E125" s="229">
         <f>E121-G121</f>
         <v>0</v>
       </c>
-      <c r="F125" s="224"/>
-      <c r="G125" s="225"/>
+      <c r="F125" s="230"/>
+      <c r="G125" s="231"/>
       <c r="I125" s="2"/>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
@@ -23298,11 +23458,11 @@
       <c r="B127" s="165"/>
       <c r="C127" s="36"/>
       <c r="D127" s="2"/>
-      <c r="E127" s="226" t="s">
+      <c r="E127" s="232" t="s">
         <v>10</v>
       </c>
-      <c r="F127" s="226"/>
-      <c r="G127" s="226"/>
+      <c r="F127" s="232"/>
+      <c r="G127" s="232"/>
       <c r="I127" s="2"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
@@ -23445,25 +23605,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="219" t="s">
+      <c r="B1" s="225" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="220"/>
-      <c r="D1" s="220"/>
-      <c r="E1" s="220"/>
-      <c r="F1" s="220"/>
-      <c r="G1" s="221"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="227"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="222" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="222"/>
-      <c r="D2" s="222"/>
-      <c r="E2" s="222"/>
-      <c r="F2" s="222"/>
+      <c r="B2" s="228" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="228"/>
+      <c r="D2" s="228"/>
+      <c r="E2" s="228"/>
+      <c r="F2" s="228"/>
       <c r="G2" s="77"/>
       <c r="H2" s="4"/>
       <c r="I2" s="2"/>
@@ -25557,12 +25717,12 @@
       <c r="B85" s="165"/>
       <c r="C85" s="36"/>
       <c r="D85" s="2"/>
-      <c r="E85" s="223">
+      <c r="E85" s="229">
         <f>E81-G81</f>
         <v>0</v>
       </c>
-      <c r="F85" s="224"/>
-      <c r="G85" s="225"/>
+      <c r="F85" s="230"/>
+      <c r="G85" s="231"/>
       <c r="I85" s="2"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
@@ -25578,11 +25738,11 @@
       <c r="B87" s="165"/>
       <c r="C87" s="36"/>
       <c r="D87" s="2"/>
-      <c r="E87" s="226" t="s">
+      <c r="E87" s="232" t="s">
         <v>10</v>
       </c>
-      <c r="F87" s="226"/>
-      <c r="G87" s="226"/>
+      <c r="F87" s="232"/>
+      <c r="G87" s="232"/>
       <c r="I87" s="2"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -25724,25 +25884,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="219" t="s">
+      <c r="B1" s="225" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="220"/>
-      <c r="D1" s="220"/>
-      <c r="E1" s="220"/>
-      <c r="F1" s="220"/>
-      <c r="G1" s="221"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="227"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="222" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="222"/>
-      <c r="D2" s="222"/>
-      <c r="E2" s="222"/>
-      <c r="F2" s="222"/>
+      <c r="B2" s="228" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="228"/>
+      <c r="D2" s="228"/>
+      <c r="E2" s="228"/>
+      <c r="F2" s="228"/>
       <c r="G2" s="77"/>
       <c r="H2" s="4"/>
       <c r="I2" s="2"/>
@@ -28575,12 +28735,12 @@
       <c r="B114" s="165"/>
       <c r="C114" s="36"/>
       <c r="D114" s="2"/>
-      <c r="E114" s="223">
+      <c r="E114" s="229">
         <f>E110-G110</f>
         <v>0</v>
       </c>
-      <c r="F114" s="224"/>
-      <c r="G114" s="225"/>
+      <c r="F114" s="230"/>
+      <c r="G114" s="231"/>
       <c r="I114" s="2"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
@@ -28596,11 +28756,11 @@
       <c r="B116" s="165"/>
       <c r="C116" s="36"/>
       <c r="D116" s="2"/>
-      <c r="E116" s="226" t="s">
+      <c r="E116" s="232" t="s">
         <v>10</v>
       </c>
-      <c r="F116" s="226"/>
-      <c r="G116" s="226"/>
+      <c r="F116" s="232"/>
+      <c r="G116" s="232"/>
       <c r="I116" s="2"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
@@ -28745,25 +28905,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="219" t="s">
+      <c r="B1" s="225" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="220"/>
-      <c r="D1" s="220"/>
-      <c r="E1" s="220"/>
-      <c r="F1" s="220"/>
-      <c r="G1" s="221"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="227"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="222" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="222"/>
-      <c r="D2" s="222"/>
-      <c r="E2" s="222"/>
-      <c r="F2" s="222"/>
+      <c r="B2" s="228" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="228"/>
+      <c r="D2" s="228"/>
+      <c r="E2" s="228"/>
+      <c r="F2" s="228"/>
       <c r="G2" s="77"/>
       <c r="H2" s="4"/>
       <c r="I2" s="2"/>
@@ -32840,12 +33000,12 @@
       <c r="B160" s="165"/>
       <c r="C160" s="36"/>
       <c r="D160" s="2"/>
-      <c r="E160" s="223">
+      <c r="E160" s="229">
         <f>E156-G156</f>
         <v>0</v>
       </c>
-      <c r="F160" s="224"/>
-      <c r="G160" s="225"/>
+      <c r="F160" s="230"/>
+      <c r="G160" s="231"/>
       <c r="I160" s="2"/>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
@@ -32861,11 +33021,11 @@
       <c r="B162" s="165"/>
       <c r="C162" s="36"/>
       <c r="D162" s="2"/>
-      <c r="E162" s="226" t="s">
+      <c r="E162" s="232" t="s">
         <v>10</v>
       </c>
-      <c r="F162" s="226"/>
-      <c r="G162" s="226"/>
+      <c r="F162" s="232"/>
+      <c r="G162" s="232"/>
       <c r="I162" s="2"/>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
@@ -32989,8 +33149,8 @@
   <dimension ref="A1:Q140"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D114" sqref="D114"/>
+      <pane ySplit="3" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H118" sqref="H118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -33009,25 +33169,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="219" t="s">
+      <c r="B1" s="225" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="220"/>
-      <c r="D1" s="220"/>
-      <c r="E1" s="220"/>
-      <c r="F1" s="220"/>
-      <c r="G1" s="221"/>
+      <c r="C1" s="226"/>
+      <c r="D1" s="226"/>
+      <c r="E1" s="226"/>
+      <c r="F1" s="226"/>
+      <c r="G1" s="227"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="222" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="222"/>
-      <c r="D2" s="222"/>
-      <c r="E2" s="222"/>
-      <c r="F2" s="222"/>
+      <c r="B2" s="228" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="228"/>
+      <c r="D2" s="228"/>
+      <c r="E2" s="228"/>
+      <c r="F2" s="228"/>
       <c r="G2" s="77"/>
       <c r="H2" s="4"/>
       <c r="I2" s="2"/>
@@ -35304,11 +35464,15 @@
       <c r="E87" s="20">
         <v>1769</v>
       </c>
-      <c r="F87" s="49"/>
-      <c r="G87" s="27"/>
+      <c r="F87" s="239">
+        <v>44480</v>
+      </c>
+      <c r="G87" s="240">
+        <v>1769</v>
+      </c>
       <c r="H87" s="28">
         <f t="shared" si="0"/>
-        <v>1769</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -36106,11 +36270,15 @@
       <c r="E118" s="27">
         <v>10697</v>
       </c>
-      <c r="F118" s="216"/>
-      <c r="G118" s="92"/>
+      <c r="F118" s="216">
+        <v>44480</v>
+      </c>
+      <c r="G118" s="92">
+        <v>10697</v>
+      </c>
       <c r="H118" s="28">
         <f t="shared" si="0"/>
-        <v>10697</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
@@ -36192,11 +36360,11 @@
       <c r="F123" s="37"/>
       <c r="G123" s="37">
         <f>SUM(G4:G122)</f>
-        <v>831376</v>
+        <v>843842</v>
       </c>
       <c r="H123" s="38">
         <f>SUM(H4:H122)</f>
-        <v>12466</v>
+        <v>0</v>
       </c>
       <c r="I123" s="2"/>
     </row>
@@ -36238,12 +36406,12 @@
       <c r="B127" s="165"/>
       <c r="C127" s="36"/>
       <c r="D127" s="2"/>
-      <c r="E127" s="223">
+      <c r="E127" s="229">
         <f>E123-G123</f>
-        <v>12466</v>
-      </c>
-      <c r="F127" s="224"/>
-      <c r="G127" s="225"/>
+        <v>0</v>
+      </c>
+      <c r="F127" s="230"/>
+      <c r="G127" s="231"/>
       <c r="I127" s="2"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
@@ -36259,11 +36427,11 @@
       <c r="B129" s="165"/>
       <c r="C129" s="36"/>
       <c r="D129" s="2"/>
-      <c r="E129" s="226" t="s">
+      <c r="E129" s="232" t="s">
         <v>10</v>
       </c>
-      <c r="F129" s="226"/>
-      <c r="G129" s="226"/>
+      <c r="F129" s="232"/>
+      <c r="G129" s="232"/>
       <c r="I129" s="2"/>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>